<commit_message>
Minor update to include flow QC for 96 well plates
</commit_message>
<xml_diff>
--- a/Data/Amp_data/Amplicon_metadata_fixed_anon.xlsx
+++ b/Data/Amp_data/Amplicon_metadata_fixed_anon.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z3283497\python\Annatina\MDS_amplicons\Data\Amp_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312F5721-E16F-410A-9CCF-E17A72EA471B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597D22A9-9A74-41A3-9174-7BD1B867DF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5F014143-920D-4DB0-A62E-146218771D3A}"/>
   </bookViews>
@@ -2075,18 +2075,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2115,12 +2109,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2438,8 +2432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94359532-EE02-4121-A9E9-E223D8D8A31C}">
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4008,7 +4002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B2180E-326F-4B11-AB1C-FE8AFAB36BB6}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>

</xml_diff>